<commit_message>
new insertion tests benchmarking
</commit_message>
<xml_diff>
--- a/tests/results/diagrams.xlsx
+++ b/tests/results/diagrams.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14740" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14740" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="insert columns" sheetId="1" r:id="rId1"/>
     <sheet name="insert rows" sheetId="2" r:id="rId2"/>
     <sheet name="scan test" sheetId="3" r:id="rId3"/>
     <sheet name="scan test 2" sheetId="4" r:id="rId4"/>
+    <sheet name="insert 5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'insert columns'!$A$1:$F$192</definedName>
@@ -23,6 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'scan test'!$A$1:$D$32</definedName>
     <definedName name="times_insert" localSheetId="0">'insert columns'!$A$2:$D$192</definedName>
     <definedName name="times_insert" localSheetId="1">'insert rows'!$A$1:$D$193</definedName>
+    <definedName name="times_insert_5" localSheetId="4">'insert 5'!$A$1:$D$33</definedName>
     <definedName name="times_scan" localSheetId="2">'scan test'!$A$1:$D$32</definedName>
     <definedName name="times_scan_2" localSheetId="3">'scan test 2'!$A$1:$D$38</definedName>
   </definedNames>
@@ -50,7 +52,17 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="times_insert1" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="2" name="times_insert_5" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/tobiaswollowski/Git/epic-battle-db/tests/results/times_insert_5.csv" decimal="," thousands="." comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="times_insert1" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/tobiaswollowski/Git/epic-battle-db/build/times_insert.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -60,7 +72,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="times_scan" type="6" refreshedVersion="0" background="1" saveData="1">
+  <connection id="4" name="times_scan" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="/Users/tobiaswollowski/Git/epic-battle-db/build/times_scan.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="4">
         <textField/>
@@ -70,8 +82,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="times_scan_2" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/tobiaswollowski/Git/epic-battle-db/tests/results/times_scan_2.csv" decimal="," thousands="." comma="1">
+  <connection id="5" name="times_scan_2" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/tobiaswollowski/Git/epic-battle-db/tests/results/times_scan_2.csv" decimal="," thousands="." comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -84,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>rows</t>
   </si>
@@ -210,6 +222,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1707,11 +1720,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2087890496"/>
-        <c:axId val="-2045486320"/>
+        <c:axId val="1116613744"/>
+        <c:axId val="1116615792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2087890496"/>
+        <c:axId val="1116613744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1754,7 +1767,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2045486320"/>
+        <c:crossAx val="1116615792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1762,7 +1775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2045486320"/>
+        <c:axId val="1116615792"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1809,6 +1822,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1868,7 +1882,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2087890496"/>
+        <c:crossAx val="1116613744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1971,6 +1985,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2451,11 +2466,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2087853152"/>
-        <c:axId val="-2087849888"/>
+        <c:axId val="1090281040"/>
+        <c:axId val="1090284304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2087853152"/>
+        <c:axId val="1090281040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2512,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2087849888"/>
+        <c:crossAx val="1090284304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2505,7 +2520,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2087849888"/>
+        <c:axId val="1090284304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2526,6 +2541,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2585,7 +2601,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2087853152"/>
+        <c:crossAx val="1090281040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2688,6 +2704,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3168,11 +3185,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2045432688"/>
-        <c:axId val="-2045429424"/>
+        <c:axId val="1090323600"/>
+        <c:axId val="1090326864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2045432688"/>
+        <c:axId val="1090323600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3215,7 +3232,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2045429424"/>
+        <c:crossAx val="1090326864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3223,7 +3240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2045429424"/>
+        <c:axId val="1090326864"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3270,6 +3287,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3329,7 +3347,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2045432688"/>
+        <c:crossAx val="1090323600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3432,7 +3450,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3962,11 +3979,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2045391360"/>
-        <c:axId val="-2045388368"/>
+        <c:axId val="1090372352"/>
+        <c:axId val="1090375344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2045391360"/>
+        <c:axId val="1090372352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4008,7 +4025,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2045388368"/>
+        <c:crossAx val="1090375344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4016,7 +4033,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2045388368"/>
+        <c:axId val="1090375344"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4067,7 +4084,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2045391360"/>
+        <c:crossAx val="1090372352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4081,7 +4098,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4188,7 +4204,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4802,11 +4817,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2087820448"/>
-        <c:axId val="-2087817456"/>
+        <c:axId val="1116643776"/>
+        <c:axId val="1116646768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2087820448"/>
+        <c:axId val="1116643776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4848,7 +4863,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2087817456"/>
+        <c:crossAx val="1116646768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4856,7 +4871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2087817456"/>
+        <c:axId val="1116646768"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4903,7 +4918,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4963,7 +4977,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2087820448"/>
+        <c:crossAx val="1116643776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5777,11 +5791,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1977505168"/>
-        <c:axId val="-1977387056"/>
+        <c:axId val="1090404704"/>
+        <c:axId val="1090407696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1977505168"/>
+        <c:axId val="1090404704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5823,7 +5837,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1977387056"/>
+        <c:crossAx val="1090407696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5831,7 +5845,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1977387056"/>
+        <c:axId val="1090407696"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5938,7 +5952,922 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1977505168"/>
+        <c:crossAx val="1090404704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>insert times log 10</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'insert 5'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>rows</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'insert 5'!$A$2:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0E6</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.0E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'insert 5'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>columns</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'insert 5'!$B$2:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>128.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>128.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'insert 5'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>time ns row store</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'insert 5'!$C$2:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>154727.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250548.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>457944.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>809444.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.751449E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.68482E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.925534E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.427056E7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.465905E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.063025E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.928647E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.737293E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1407276E7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.5064737E7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.9179602E7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.20881931E8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5586307E7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5640436E7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.3082305E7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.2718188E7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.72682419E8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.21828179E8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.65501677E8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.177243846E9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.44247025E8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.16567485E8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.33952302E8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.00583818E8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.669610514E9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.086104072E9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.472902193E9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.4019349069E10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'insert 5'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> time ns col store</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'insert 5'!$D$2:$D$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>150687.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>245398.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>407599.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>760965.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.084969E6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.191693E6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.502476E6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3642793E7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.390489E6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.037878E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.585513E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.672413E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1702356E7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.2041173E7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.3198691E7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.32713594E8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6929671E7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1140951E7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0667203E7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.7500585E7</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.88413044E8</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.30064916E8</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.58537841E8</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2031513E9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.42970209E8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.07294945E8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.33326423E8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7.95151588E8</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.690094804E9</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.77082698E9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.726094553E9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5722238615E10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1285608080"/>
+        <c:axId val="1285617152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1285608080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1285617152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1285617152"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>nanoseconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1285608080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6266,6 +7195,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -8808,6 +9777,509 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9510,20 +10982,59 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_scan" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_scan" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_scan_2" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_scan_2" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert_5" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15718,7 +17229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
+    <sheetView zoomScale="50" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -16266,4 +17777,488 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10000</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>154727</v>
+      </c>
+      <c r="D2">
+        <v>150687</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>10000</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>250548</v>
+      </c>
+      <c r="D3">
+        <v>245398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>10000</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>457944</v>
+      </c>
+      <c r="D4">
+        <v>407599</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10000</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>809444</v>
+      </c>
+      <c r="D5">
+        <v>760965</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>10000</v>
+      </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>1751449</v>
+      </c>
+      <c r="D6">
+        <v>2084969</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>10000</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>3684820</v>
+      </c>
+      <c r="D7">
+        <v>3191693</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>10000</v>
+      </c>
+      <c r="B8">
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <v>6925534</v>
+      </c>
+      <c r="D8">
+        <v>8502476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>10000</v>
+      </c>
+      <c r="B9">
+        <v>128</v>
+      </c>
+      <c r="C9">
+        <v>14270560</v>
+      </c>
+      <c r="D9">
+        <v>13642793</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>100000</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1465905</v>
+      </c>
+      <c r="D10">
+        <v>1390489</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>100000</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2063025</v>
+      </c>
+      <c r="D11">
+        <v>2037878</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>100000</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4928647</v>
+      </c>
+      <c r="D12">
+        <v>3585513</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>100000</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>7737293</v>
+      </c>
+      <c r="D13">
+        <v>7672413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>100000</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>21407276</v>
+      </c>
+      <c r="D14">
+        <v>21702356</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>100000</v>
+      </c>
+      <c r="B15">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>35064737</v>
+      </c>
+      <c r="D15">
+        <v>32041173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>100000</v>
+      </c>
+      <c r="B16">
+        <v>64</v>
+      </c>
+      <c r="C16">
+        <v>69179602</v>
+      </c>
+      <c r="D16">
+        <v>63198691</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>100000</v>
+      </c>
+      <c r="B17">
+        <v>128</v>
+      </c>
+      <c r="C17">
+        <v>120881931</v>
+      </c>
+      <c r="D17">
+        <v>132713594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1000000</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>15586307</v>
+      </c>
+      <c r="D18">
+        <v>16929671</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1000000</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>25640436</v>
+      </c>
+      <c r="D19">
+        <v>31140951</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1000000</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>43082305</v>
+      </c>
+      <c r="D20">
+        <v>40667203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1000000</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>72718188</v>
+      </c>
+      <c r="D21">
+        <v>67500585</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1000000</v>
+      </c>
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>172682419</v>
+      </c>
+      <c r="D22">
+        <v>188413044</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1000000</v>
+      </c>
+      <c r="B23">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>321828179</v>
+      </c>
+      <c r="D23">
+        <v>330064916</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1000000</v>
+      </c>
+      <c r="B24">
+        <v>64</v>
+      </c>
+      <c r="C24">
+        <v>665501677</v>
+      </c>
+      <c r="D24">
+        <v>658537841</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1000000</v>
+      </c>
+      <c r="B25">
+        <v>128</v>
+      </c>
+      <c r="C25">
+        <v>1177243846</v>
+      </c>
+      <c r="D25">
+        <v>1203151300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>10000000</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>144247025</v>
+      </c>
+      <c r="D26">
+        <v>142970209</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>10000000</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>216567485</v>
+      </c>
+      <c r="D27">
+        <v>207294945</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>10000000</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>433952302</v>
+      </c>
+      <c r="D28">
+        <v>433326423</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>10000000</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>800583818</v>
+      </c>
+      <c r="D29">
+        <v>795151588</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>10000000</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>1669610514</v>
+      </c>
+      <c r="D30">
+        <v>1690094804</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>10000000</v>
+      </c>
+      <c r="B31">
+        <v>32</v>
+      </c>
+      <c r="C31">
+        <v>3086104072</v>
+      </c>
+      <c r="D31">
+        <v>3770826980</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>10000000</v>
+      </c>
+      <c r="B32">
+        <v>64</v>
+      </c>
+      <c r="C32">
+        <v>6472902193</v>
+      </c>
+      <c r="D32">
+        <v>7726094553</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>10000000</v>
+      </c>
+      <c r="B33">
+        <v>128</v>
+      </c>
+      <c r="C33">
+        <v>14019349069</v>
+      </c>
+      <c r="D33">
+        <v>15722238615</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add inserts per second metrik
</commit_message>
<xml_diff>
--- a/tests/results/diagrams.xlsx
+++ b/tests/results/diagrams.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="insert columns" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'insert rows'!$A$1:$D$193</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'scan test'!$A$1:$D$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Tabelle1!$A$1:$D$33</definedName>
-    <definedName name="times_insert" localSheetId="9">'Compare Inserts (32bit)'!$A$1:$H$9</definedName>
+    <definedName name="times_insert" localSheetId="9">'Compare Inserts (32bit)'!$A$2:$H$10</definedName>
     <definedName name="times_insert" localSheetId="10">'Compare Inserts (64bit)'!$A$1:$H$9</definedName>
     <definedName name="times_insert" localSheetId="0">'insert columns'!$A$2:$D$192</definedName>
     <definedName name="times_insert" localSheetId="1">'insert rows'!$A$1:$D$193</definedName>
     <definedName name="times_insert" localSheetId="5">'O2-insert'!$A$1:$D$33</definedName>
     <definedName name="times_insert" localSheetId="7">'O3-insert'!$A$1:$D$33</definedName>
-    <definedName name="times_insert_1" localSheetId="9">'Compare Inserts (32bit)'!$A$59:$H$67</definedName>
+    <definedName name="times_insert_1" localSheetId="9">'Compare Inserts (32bit)'!$A$60:$H$68</definedName>
     <definedName name="times_insert_1" localSheetId="10">'Compare Inserts (64bit)'!$A$59:$H$67</definedName>
     <definedName name="times_insert_1" localSheetId="12">Tabelle1!$A$1:$D$33</definedName>
-    <definedName name="times_insert_2" localSheetId="9">'Compare Inserts (32bit)'!$A$70:$H$78</definedName>
+    <definedName name="times_insert_2" localSheetId="9">'Compare Inserts (32bit)'!$A$71:$H$79</definedName>
     <definedName name="times_insert_2" localSheetId="10">'Compare Inserts (64bit)'!$A$70:$H$78</definedName>
     <definedName name="times_insert_5" localSheetId="4">'insert 5'!$A$1:$D$33</definedName>
     <definedName name="times_scan" localSheetId="11">'Compate Scan (64bit)'!$A$1:$D$9</definedName>
@@ -255,7 +255,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t>rows</t>
   </si>
@@ -343,13 +343,30 @@
   <si>
     <t>col store (inlined insert)</t>
   </si>
+  <si>
+    <t>RAW data</t>
+  </si>
+  <si>
+    <t>Fields per Second</t>
+  </si>
+  <si>
+    <t>=(ROWS * COLS) / TIME * 1.000.000.000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -377,10 +394,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1938,11 +1957,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2056338000"/>
-        <c:axId val="2141329696"/>
+        <c:axId val="-2138240512"/>
+        <c:axId val="-2138237200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2056338000"/>
+        <c:axId val="-2138240512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1985,7 +2004,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141329696"/>
+        <c:crossAx val="-2138237200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1993,7 +2012,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141329696"/>
+        <c:axId val="-2138237200"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2100,7 +2119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056338000"/>
+        <c:crossAx val="-2138240512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2853,11 +2872,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2144406560"/>
-        <c:axId val="2144424192"/>
+        <c:axId val="-2137296192"/>
+        <c:axId val="-2137293104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2144406560"/>
+        <c:axId val="-2137296192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2899,7 +2918,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144424192"/>
+        <c:crossAx val="-2137293104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2907,7 +2926,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2144424192"/>
+        <c:axId val="-2137293104"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3014,7 +3033,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2144406560"/>
+        <c:crossAx val="-2137296192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3767,11 +3786,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2127996896"/>
-        <c:axId val="-2127896336"/>
+        <c:axId val="-2136722768"/>
+        <c:axId val="-2136719632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2127996896"/>
+        <c:axId val="-2136722768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3813,7 +3832,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127896336"/>
+        <c:crossAx val="-2136719632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3821,7 +3840,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127896336"/>
+        <c:axId val="-2136719632"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3927,7 +3946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127996896"/>
+        <c:crossAx val="-2136722768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4055,6 +4074,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4095,7 +4115,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$C$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4130,7 +4150,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4163,7 +4183,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$C$2:$C$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4201,7 +4221,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$D$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4236,7 +4256,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4269,7 +4289,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$D$2:$D$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4307,7 +4327,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$E$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4342,7 +4362,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4375,7 +4395,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$E$2:$E$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4413,7 +4433,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$F$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4448,7 +4468,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4481,7 +4501,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$F$2:$F$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4519,7 +4539,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$G$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4554,7 +4574,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4587,7 +4607,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$G$2:$G$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4625,7 +4645,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$H$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4660,7 +4680,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4693,7 +4713,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$H$2:$H$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4736,11 +4756,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2058571120"/>
-        <c:axId val="-2058928384"/>
+        <c:axId val="-2137277200"/>
+        <c:axId val="-2137274160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2058571120"/>
+        <c:axId val="-2137277200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4783,7 +4803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058928384"/>
+        <c:crossAx val="-2137274160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4791,7 +4811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2058928384"/>
+        <c:axId val="-2137274160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4842,6 +4862,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4902,7 +4923,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058571120"/>
+        <c:crossAx val="-2137277200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5030,6 +5051,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5070,7 +5092,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$C$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5105,7 +5127,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5138,7 +5160,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$C$2:$C$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5176,7 +5198,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$D$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5211,7 +5233,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5244,7 +5266,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$D$2:$D$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$D$3:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5282,7 +5304,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$E$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5317,7 +5339,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5350,7 +5372,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$E$2:$E$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$E$3:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5388,7 +5410,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$F$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5423,7 +5445,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5456,7 +5478,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$F$2:$F$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$F$3:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5494,7 +5516,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$G$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5529,7 +5551,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5562,7 +5584,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$G$2:$G$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$G$3:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5600,7 +5622,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$H$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5635,7 +5657,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$2:$B$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5668,7 +5690,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$H$2:$H$9</c:f>
+              <c:f>'Compare Inserts (32bit)'!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -5711,11 +5733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2057199936"/>
-        <c:axId val="-2056976144"/>
+        <c:axId val="-2137181872"/>
+        <c:axId val="-2137178832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2057199936"/>
+        <c:axId val="-2137181872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5758,7 +5780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056976144"/>
+        <c:crossAx val="-2137178832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5766,7 +5788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2056976144"/>
+        <c:axId val="-2137178832"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -5819,6 +5841,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5879,7 +5902,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057199936"/>
+        <c:crossAx val="-2137181872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6047,7 +6070,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$C$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6082,7 +6105,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$23:$B$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$24:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6115,7 +6138,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$C$23:$C$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$C$24:$C$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6153,7 +6176,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$D$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6188,7 +6211,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$23:$B$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$24:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6221,7 +6244,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$D$23:$D$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$D$24:$D$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6259,7 +6282,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$E$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6294,7 +6317,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$23:$B$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$24:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6327,7 +6350,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$E$23:$E$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$E$24:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6365,7 +6388,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$F$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6400,7 +6423,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$23:$B$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$24:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6433,7 +6456,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$F$23:$F$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$F$24:$F$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6471,7 +6494,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$G$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$G$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6506,7 +6529,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$23:$B$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$24:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6539,7 +6562,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$G$23:$G$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$G$24:$G$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6577,7 +6600,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Compare Inserts (32bit)'!$H$1</c:f>
+              <c:f>'Compare Inserts (32bit)'!$H$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6612,7 +6635,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$B$23:$B$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$B$24:$B$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6645,7 +6668,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compare Inserts (32bit)'!$H$23:$H$30</c:f>
+              <c:f>'Compare Inserts (32bit)'!$H$24:$H$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6688,11 +6711,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2058745328"/>
-        <c:axId val="-2058533360"/>
+        <c:axId val="-2137116624"/>
+        <c:axId val="-2137113520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2058745328"/>
+        <c:axId val="-2137116624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6735,7 +6758,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058533360"/>
+        <c:crossAx val="-2137113520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6743,7 +6766,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2058533360"/>
+        <c:axId val="-2137113520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6849,7 +6872,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058745328"/>
+        <c:crossAx val="-2137116624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7659,11 +7682,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2059106768"/>
-        <c:axId val="-2128114784"/>
+        <c:axId val="-2136654848"/>
+        <c:axId val="-2136651808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2059106768"/>
+        <c:axId val="-2136654848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7706,7 +7729,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128114784"/>
+        <c:crossAx val="-2136651808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7714,7 +7737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128114784"/>
+        <c:axId val="-2136651808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7826,7 +7849,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2059106768"/>
+        <c:crossAx val="-2136654848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8636,11 +8659,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2056679376"/>
-        <c:axId val="-2056676400"/>
+        <c:axId val="-2137800240"/>
+        <c:axId val="-2137803296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2056679376"/>
+        <c:axId val="-2137800240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8683,7 +8706,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056676400"/>
+        <c:crossAx val="-2137803296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8691,7 +8714,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2056676400"/>
+        <c:axId val="-2137803296"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -8805,7 +8828,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056679376"/>
+        <c:crossAx val="-2137800240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9615,11 +9638,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2058172288"/>
-        <c:axId val="-2058269296"/>
+        <c:axId val="-2137865472"/>
+        <c:axId val="-2137868528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2058172288"/>
+        <c:axId val="-2137865472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9662,7 +9685,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058269296"/>
+        <c:crossAx val="-2137868528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9670,7 +9693,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2058269296"/>
+        <c:axId val="-2137868528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9777,7 +9800,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058172288"/>
+        <c:crossAx val="-2137865472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10168,11 +10191,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2058449888"/>
-        <c:axId val="-2059234784"/>
+        <c:axId val="2131886704"/>
+        <c:axId val="2131883664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2058449888"/>
+        <c:axId val="2131886704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10214,7 +10237,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2059234784"/>
+        <c:crossAx val="2131883664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10222,7 +10245,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2059234784"/>
+        <c:axId val="2131883664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10328,7 +10351,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058449888"/>
+        <c:crossAx val="2131886704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10719,11 +10742,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2078175616"/>
-        <c:axId val="-2078202352"/>
+        <c:axId val="2131812256"/>
+        <c:axId val="2131809216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2078175616"/>
+        <c:axId val="2131812256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10765,7 +10788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078202352"/>
+        <c:crossAx val="2131809216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10773,7 +10796,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2078202352"/>
+        <c:axId val="2131809216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10879,7 +10902,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078175616"/>
+        <c:crossAx val="2131812256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11462,11 +11485,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2127898144"/>
-        <c:axId val="-2127887776"/>
+        <c:axId val="-2138092944"/>
+        <c:axId val="-2138089552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2127898144"/>
+        <c:axId val="-2138092944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11508,7 +11531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127887776"/>
+        <c:crossAx val="-2138089552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11516,7 +11539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127887776"/>
+        <c:axId val="-2138089552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11596,7 +11619,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127898144"/>
+        <c:crossAx val="-2138092944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12132,11 +12155,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2056516832"/>
-        <c:axId val="-2056513808"/>
+        <c:axId val="-2136689808"/>
+        <c:axId val="-2136633856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2056516832"/>
+        <c:axId val="-2136689808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12178,7 +12201,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056513808"/>
+        <c:crossAx val="-2136633856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12186,7 +12209,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2056513808"/>
+        <c:axId val="-2136633856"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -12237,7 +12260,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056516832"/>
+        <c:crossAx val="-2136689808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12765,11 +12788,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2064617824"/>
-        <c:axId val="-2064614624"/>
+        <c:axId val="-2137932080"/>
+        <c:axId val="-2137935216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2064617824"/>
+        <c:axId val="-2137932080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12811,7 +12834,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2064614624"/>
+        <c:crossAx val="-2137935216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12819,7 +12842,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2064614624"/>
+        <c:axId val="-2137935216"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -12901,7 +12924,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2064617824"/>
+        <c:crossAx val="-2137932080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13484,11 +13507,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2142097040"/>
-        <c:axId val="2142057168"/>
+        <c:axId val="2131956464"/>
+        <c:axId val="2131953056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2142097040"/>
+        <c:axId val="2131956464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13531,7 +13554,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142057168"/>
+        <c:crossAx val="2131953056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13539,7 +13562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142057168"/>
+        <c:axId val="2131953056"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -13645,7 +13668,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2142097040"/>
+        <c:crossAx val="2131956464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14277,11 +14300,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2059736288"/>
-        <c:axId val="-2060444320"/>
+        <c:axId val="-2137491632"/>
+        <c:axId val="-2137488544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2059736288"/>
+        <c:axId val="-2137491632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14323,7 +14346,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2060444320"/>
+        <c:crossAx val="-2137488544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14331,7 +14354,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2060444320"/>
+        <c:axId val="-2137488544"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -14383,7 +14406,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2059736288"/>
+        <c:crossAx val="-2137491632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15116,11 +15139,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2128056176"/>
-        <c:axId val="-2128000048"/>
+        <c:axId val="2131993200"/>
+        <c:axId val="-2137405648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2128056176"/>
+        <c:axId val="2131993200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15162,7 +15185,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128000048"/>
+        <c:crossAx val="-2137405648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15170,7 +15193,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128000048"/>
+        <c:axId val="-2137405648"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -15246,6 +15269,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -15276,7 +15300,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2128056176"/>
+        <c:crossAx val="2131993200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16089,11 +16113,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2056727552"/>
-        <c:axId val="-2057984336"/>
+        <c:axId val="-2138846912"/>
+        <c:axId val="-2138113312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2056727552"/>
+        <c:axId val="-2138846912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16135,7 +16159,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2057984336"/>
+        <c:crossAx val="-2138113312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16143,7 +16167,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2057984336"/>
+        <c:axId val="-2138113312"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -16249,7 +16273,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056727552"/>
+        <c:crossAx val="-2138846912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17002,11 +17026,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2058373680"/>
-        <c:axId val="-2058737760"/>
+        <c:axId val="-2138969744"/>
+        <c:axId val="-2138972896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2058373680"/>
+        <c:axId val="-2138969744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17048,7 +17072,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058737760"/>
+        <c:crossAx val="-2138972896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17056,7 +17080,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2058737760"/>
+        <c:axId val="-2138972896"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -17162,7 +17186,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058373680"/>
+        <c:crossAx val="-2138969744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17915,11 +17939,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2059694688"/>
-        <c:axId val="-2127881424"/>
+        <c:axId val="-2139038240"/>
+        <c:axId val="-2139041344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2059694688"/>
+        <c:axId val="-2139038240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17961,7 +17985,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2127881424"/>
+        <c:crossAx val="-2139041344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17969,7 +17993,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2127881424"/>
+        <c:axId val="-2139041344"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -18075,7 +18099,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2059694688"/>
+        <c:crossAx val="-2139038240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18828,11 +18852,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2058629168"/>
-        <c:axId val="-2058633664"/>
+        <c:axId val="-2137378880"/>
+        <c:axId val="-2137375744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2058629168"/>
+        <c:axId val="-2137378880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18874,7 +18898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058633664"/>
+        <c:crossAx val="-2137375744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18882,7 +18906,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2058633664"/>
+        <c:axId val="-2137375744"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -18988,7 +19012,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2058629168"/>
+        <c:crossAx val="-2137378880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -30546,13 +30570,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>355599</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>118534</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>728133</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>16934</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -30578,13 +30602,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>433659</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>30975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>806193</xdr:colOff>
-      <xdr:row>77</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>146203</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -30610,13 +30634,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>18406</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>48</xdr:col>
       <xdr:colOff>372535</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>117332</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -31219,19 +31243,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert_2" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert_1" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert_2" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert_2" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert_1" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="times_insert_2" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34263,10 +34287,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView zoomScale="74" zoomScaleNormal="41" zoomScalePageLayoutView="41" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView topLeftCell="A13" zoomScale="74" zoomScaleNormal="41" zoomScalePageLayoutView="41" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34282,55 +34306,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>100000</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1587403</v>
-      </c>
-      <c r="D2">
-        <v>1669745</v>
-      </c>
-      <c r="E2">
-        <v>338773</v>
-      </c>
-      <c r="F2">
-        <v>848271</v>
-      </c>
-      <c r="G2">
-        <v>1661601</v>
-      </c>
-      <c r="H2">
-        <v>320876</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -34338,25 +34341,25 @@
         <v>100000</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1640509</v>
+        <v>1587403</v>
       </c>
       <c r="D3">
-        <v>2322927</v>
+        <v>1669745</v>
       </c>
       <c r="E3">
-        <v>536641</v>
+        <v>338773</v>
       </c>
       <c r="F3">
-        <v>944621</v>
+        <v>848271</v>
       </c>
       <c r="G3">
-        <v>2400658</v>
+        <v>1661601</v>
       </c>
       <c r="H3">
-        <v>524517</v>
+        <v>320876</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -34364,25 +34367,25 @@
         <v>100000</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>1764156</v>
+        <v>1640509</v>
       </c>
       <c r="D4">
-        <v>4527444</v>
+        <v>2322927</v>
       </c>
       <c r="E4">
-        <v>961910</v>
+        <v>536641</v>
       </c>
       <c r="F4">
-        <v>1025142</v>
+        <v>944621</v>
       </c>
       <c r="G4">
-        <v>3705243</v>
+        <v>2400658</v>
       </c>
       <c r="H4">
-        <v>987366</v>
+        <v>524517</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -34390,25 +34393,25 @@
         <v>100000</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>1737417</v>
+        <v>1764156</v>
       </c>
       <c r="D5">
-        <v>7617014</v>
+        <v>4527444</v>
       </c>
       <c r="E5">
-        <v>1918697</v>
+        <v>961910</v>
       </c>
       <c r="F5">
-        <v>914026</v>
+        <v>1025142</v>
       </c>
       <c r="G5">
-        <v>7345545</v>
+        <v>3705243</v>
       </c>
       <c r="H5">
-        <v>1955217</v>
+        <v>987366</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -34416,25 +34419,25 @@
         <v>100000</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>1776439</v>
+        <v>1737417</v>
       </c>
       <c r="D6">
-        <v>12670200</v>
+        <v>7617014</v>
       </c>
       <c r="E6">
-        <v>3910421</v>
+        <v>1918697</v>
       </c>
       <c r="F6">
-        <v>1259810</v>
+        <v>914026</v>
       </c>
       <c r="G6">
-        <v>12444252</v>
+        <v>7345545</v>
       </c>
       <c r="H6">
-        <v>4235425</v>
+        <v>1955217</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -34442,25 +34445,25 @@
         <v>100000</v>
       </c>
       <c r="B7">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>2837372</v>
+        <v>1776439</v>
       </c>
       <c r="D7">
-        <v>23052823</v>
+        <v>12670200</v>
       </c>
       <c r="E7">
-        <v>8699730</v>
+        <v>3910421</v>
       </c>
       <c r="F7">
-        <v>2336760</v>
+        <v>1259810</v>
       </c>
       <c r="G7">
-        <v>28357708</v>
+        <v>12444252</v>
       </c>
       <c r="H7">
-        <v>10742689</v>
+        <v>4235425</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -34468,25 +34471,25 @@
         <v>100000</v>
       </c>
       <c r="B8">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C8">
-        <v>18435381</v>
+        <v>2837372</v>
       </c>
       <c r="D8">
-        <v>44781703</v>
+        <v>23052823</v>
       </c>
       <c r="E8">
-        <v>18237650</v>
+        <v>8699730</v>
       </c>
       <c r="F8">
-        <v>16728171</v>
+        <v>2336760</v>
       </c>
       <c r="G8">
-        <v>82013530</v>
+        <v>28357708</v>
       </c>
       <c r="H8">
-        <v>51476258</v>
+        <v>10742689</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -34494,137 +34497,129 @@
         <v>100000</v>
       </c>
       <c r="B9">
+        <v>64</v>
+      </c>
+      <c r="C9">
+        <v>18435381</v>
+      </c>
+      <c r="D9">
+        <v>44781703</v>
+      </c>
+      <c r="E9">
+        <v>18237650</v>
+      </c>
+      <c r="F9">
+        <v>16728171</v>
+      </c>
+      <c r="G9">
+        <v>82013530</v>
+      </c>
+      <c r="H9">
+        <v>51476258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>100000</v>
+      </c>
+      <c r="B10">
         <v>128</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>24503890</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>86560831</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>33422579</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>23728559</v>
       </c>
-      <c r="G9">
+      <c r="G10">
         <v>173527057</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>124354571</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="1" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <f>A2</f>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f>A3</f>
         <v>100000</v>
       </c>
-      <c r="B13">
-        <f>B2</f>
+      <c r="B14">
+        <f>B3</f>
         <v>1</v>
       </c>
-      <c r="C13">
-        <f>($A2*$B2*4)/C2</f>
+      <c r="C14">
+        <f>($A3*$B3*4)/C3</f>
         <v>0.25198390074858118</v>
       </c>
-      <c r="D13">
-        <f t="shared" ref="D13:H20" si="0">($A2*$B2*4)/D2</f>
+      <c r="D14">
+        <f t="shared" ref="D14:H21" si="0">($A3*$B3*4)/D3</f>
         <v>0.23955753722873852</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <f t="shared" si="0"/>
         <v>1.1807316403609496</v>
       </c>
-      <c r="F13">
+      <c r="F14">
         <f t="shared" si="0"/>
         <v>0.47154741821894181</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <f t="shared" si="0"/>
         <v>0.24073167986779015</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>1.2465874668096086</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <f t="shared" ref="A14:B20" si="1">A3</f>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" ref="A15:B21" si="1">A4</f>
         <v>100000</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="C14">
-        <f t="shared" ref="C14:C20" si="2">(A3*B3*4)/C3</f>
+      <c r="C15">
+        <f t="shared" ref="C15:C21" si="2">(A4*B4*4)/C4</f>
         <v>0.48765352704556941</v>
       </c>
-      <c r="D14">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>0.34439308682537162</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>1.4907545267692928</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <f t="shared" si="0"/>
         <v>0.8469005029530362</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <f t="shared" si="0"/>
         <v>0.33324196949336388</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>1.5252127195114744</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <f t="shared" si="1"/>
-        <v>100000</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="2"/>
-        <v>0.90694927205984055</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0.35340028501732984</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="0"/>
-        <v>1.663357278747492</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>1.5607593874799783</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="0"/>
-        <v>0.43182053106908236</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="0"/>
-        <v>1.6204730565970471</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -34634,31 +34629,31 @@
       </c>
       <c r="B16">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <f t="shared" si="2"/>
-        <v>1.8418146017910495</v>
+        <v>0.90694927205984055</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0.42011213317974733</v>
+        <v>0.35340028501732984</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>1.6677985111771165</v>
+        <v>1.663357278747492</v>
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>3.5009945012505113</v>
+        <v>1.5607593874799783</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
-        <v>0.43563819975236689</v>
+        <v>0.43182053106908236</v>
       </c>
       <c r="H16">
         <f t="shared" si="0"/>
-        <v>1.6366469808722</v>
+        <v>1.6204730565970471</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -34668,31 +34663,31 @@
       </c>
       <c r="B17">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <f t="shared" si="2"/>
-        <v>3.6027130681098534</v>
+        <v>1.8418146017910495</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>0.50512225537087019</v>
+        <v>0.42011213317974733</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
-        <v>1.6366524218236349</v>
+        <v>1.6677985111771165</v>
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>5.0801311308848156</v>
+        <v>3.5009945012505113</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
-        <v>0.51429366746992911</v>
+        <v>0.43563819975236689</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>1.5110644150232857</v>
+        <v>1.6366469808722</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -34702,31 +34697,31 @@
       </c>
       <c r="B18">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <f t="shared" si="2"/>
-        <v>4.5112167174413509</v>
+        <v>3.6027130681098534</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>0.55524653097800647</v>
+        <v>0.50512225537087019</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>1.4713100291618246</v>
+        <v>1.6366524218236349</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>5.4776699361509102</v>
+        <v>5.0801311308848156</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>0.45137639473542784</v>
+        <v>0.51429366746992911</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>1.1915080107038378</v>
+        <v>1.5110644150232857</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -34736,31 +34731,31 @@
       </c>
       <c r="B19">
         <f t="shared" si="1"/>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <f t="shared" si="2"/>
-        <v>1.3886341703488525</v>
+        <v>4.5112167174413509</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>0.57166204688553268</v>
+        <v>0.55524653097800647</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>1.4036896200990807</v>
+        <v>1.4713100291618246</v>
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>1.5303526010105946</v>
+        <v>5.4776699361509102</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>0.31214361825420756</v>
+        <v>0.45137639473542784</v>
       </c>
       <c r="H19">
         <f t="shared" si="0"/>
-        <v>0.49731664644310392</v>
+        <v>1.1915080107038378</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -34770,138 +34765,138 @@
       </c>
       <c r="B20">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C20">
         <f t="shared" si="2"/>
-        <v>2.0894641626288726</v>
+        <v>1.3886341703488525</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>0.59149154887387811</v>
+        <v>0.57166204688553268</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>1.5318985408038082</v>
+        <v>1.4036896200990807</v>
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>2.1577374336132253</v>
+        <v>1.5303526010105946</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>0.29505485130194997</v>
+        <v>0.31214361825420756</v>
       </c>
       <c r="H20">
         <f t="shared" si="0"/>
+        <v>0.49731664644310392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>2.0894641626288726</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>0.59149154887387811</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1.5318985408038082</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>2.1577374336132253</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>0.29505485130194997</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
         <v>0.41172591878428016</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <f>A13</f>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f>A14</f>
         <v>100000</v>
       </c>
-      <c r="B23">
-        <f>B13</f>
+      <c r="B24">
+        <f>B14</f>
         <v>1</v>
       </c>
-      <c r="C23" s="2">
-        <f>C13*1000000/1048576</f>
+      <c r="C24" s="2">
+        <f>C14*1000000/1048576</f>
         <v>0.24031057429178351</v>
       </c>
-      <c r="D23" s="2">
-        <f t="shared" ref="D23:H23" si="3">D13*1000000/1048576</f>
+      <c r="D24" s="2">
+        <f t="shared" ref="D24:H24" si="3">D14*1000000/1048576</f>
         <v>0.22845987055658198</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E24" s="2">
         <f t="shared" si="3"/>
         <v>1.1260334399804588</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F24" s="2">
         <f t="shared" si="3"/>
         <v>0.44970266172308138</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G24" s="2">
         <f t="shared" si="3"/>
         <v>0.22957962023524298</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H24" s="2">
         <f t="shared" si="3"/>
         <v>1.1888384502502525</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <f t="shared" ref="A24:B30" si="4">A14</f>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="shared" ref="A25:B31" si="4">A15</f>
         <v>100000</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="C24" s="2">
-        <f t="shared" ref="C24:H30" si="5">C14*1000000/1048576</f>
+      <c r="C25" s="2">
+        <f t="shared" ref="C25:H31" si="5">C15*1000000/1048576</f>
         <v>0.46506264404828018</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D25" s="2">
         <f t="shared" si="5"/>
         <v>0.32843884165322457</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E25" s="2">
         <f t="shared" si="5"/>
         <v>1.421694304246228</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F25" s="2">
         <f t="shared" si="5"/>
         <v>0.80766725821784613</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G25" s="2">
         <f t="shared" si="5"/>
         <v>0.3178043074544562</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H25" s="2">
         <f t="shared" si="5"/>
         <v>1.4545561976542229</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <f t="shared" si="4"/>
-        <v>100000</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="C25" s="2">
-        <f t="shared" si="5"/>
-        <v>0.86493422704681444</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" si="5"/>
-        <v>0.33702877523167596</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" si="5"/>
-        <v>1.5863011157488747</v>
-      </c>
-      <c r="F25" s="2">
-        <f t="shared" si="5"/>
-        <v>1.4884561419296058</v>
-      </c>
-      <c r="G25" s="2">
-        <f t="shared" si="5"/>
-        <v>0.41181614977749098</v>
-      </c>
-      <c r="H25" s="2">
-        <f t="shared" si="5"/>
-        <v>1.5454035345049353</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -34911,31 +34906,31 @@
       </c>
       <c r="B26">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C26" s="2">
         <f t="shared" si="5"/>
-        <v>1.7564912813101288</v>
+        <v>0.86493422704681444</v>
       </c>
       <c r="D26" s="2">
         <f t="shared" si="5"/>
-        <v>0.40065015142416699</v>
+        <v>0.33702877523167596</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="5"/>
-        <v>1.5905366050501981</v>
+        <v>1.5863011157488747</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="5"/>
-        <v>3.3388085377221213</v>
+        <v>1.4884561419296058</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="5"/>
-        <v>0.41545696234928786</v>
+        <v>0.41181614977749098</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="5"/>
-        <v>1.5608281906816481</v>
+        <v>1.5454035345049353</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -34945,31 +34940,31 @@
       </c>
       <c r="B27">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C27" s="2">
         <f t="shared" si="5"/>
-        <v>3.4358149224375278</v>
+        <v>1.7564912813101288</v>
       </c>
       <c r="D27" s="2">
         <f t="shared" si="5"/>
-        <v>0.48172212159239786</v>
+        <v>0.40065015142416699</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="5"/>
-        <v>1.5608333795772886</v>
+        <v>1.5905366050501981</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="5"/>
-        <v>4.8447905835006866</v>
+        <v>3.3388085377221213</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" si="5"/>
-        <v>0.49046866175644788</v>
+        <v>0.41545696234928786</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="5"/>
-        <v>1.441063323043142</v>
+        <v>1.5608281906816481</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -34979,31 +34974,31 @@
       </c>
       <c r="B28">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C28" s="2">
         <f t="shared" si="5"/>
-        <v>4.3022315191663276</v>
+        <v>3.4358149224375278</v>
       </c>
       <c r="D28" s="2">
         <f t="shared" si="5"/>
-        <v>0.52952435586739199</v>
+        <v>0.48172212159239786</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="5"/>
-        <v>1.4031505862825628</v>
+        <v>1.5608333795772886</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="5"/>
-        <v>5.2239131318577865</v>
+        <v>4.8447905835006866</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="5"/>
-        <v>0.43046607469122683</v>
+        <v>0.49046866175644788</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="5"/>
-        <v>1.1363105876005533</v>
+        <v>1.441063323043142</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -35013,31 +35008,31 @@
       </c>
       <c r="B29">
         <f t="shared" si="4"/>
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C29" s="2">
         <f t="shared" si="5"/>
-        <v>1.3243047431458019</v>
+        <v>4.3022315191663276</v>
       </c>
       <c r="D29" s="2">
         <f t="shared" si="5"/>
-        <v>0.54517941177895801</v>
+        <v>0.52952435586739199</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="5"/>
-        <v>1.3386627388945396</v>
+        <v>1.4031505862825628</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="5"/>
-        <v>1.4594579706293054</v>
+        <v>5.2239131318577865</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" si="5"/>
-        <v>0.29768335175915484</v>
+        <v>0.43046607469122683</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" si="5"/>
-        <v>0.47427811283407584</v>
+        <v>1.1363105876005533</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -35047,31 +35042,347 @@
       </c>
       <c r="B30">
         <f t="shared" si="4"/>
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="C30" s="2">
         <f t="shared" si="5"/>
-        <v>1.9926683069504476</v>
+        <v>1.3243047431458019</v>
       </c>
       <c r="D30" s="2">
         <f t="shared" si="5"/>
-        <v>0.56409029853236969</v>
+        <v>0.54517941177895801</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="5"/>
-        <v>1.4609322937048037</v>
+        <v>1.3386627388945396</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="5"/>
-        <v>2.0577787719852689</v>
+        <v>1.4594579706293054</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" si="5"/>
-        <v>0.2813862336177349</v>
+        <v>0.29768335175915484</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="5"/>
+        <v>0.47427811283407584</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f t="shared" si="4"/>
+        <v>100000</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="5"/>
+        <v>1.9926683069504476</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="5"/>
+        <v>0.56409029853236969</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="5"/>
+        <v>1.4609322937048037</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="5"/>
+        <v>2.0577787719852689</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="5"/>
+        <v>0.2813862336177349</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="5"/>
         <v>0.39265243414333362</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C33" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f>A24</f>
+        <v>100000</v>
+      </c>
+      <c r="B35">
+        <f>B24</f>
+        <v>1</v>
+      </c>
+      <c r="C35" s="4">
+        <f>($A35*$B35)/C3*1000000000</f>
+        <v>62995975.187145293</v>
+      </c>
+      <c r="D35" s="4">
+        <f t="shared" ref="D35:H35" si="6">($A35*$B35)/D3*1000000000</f>
+        <v>59889384.307184629</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" si="6"/>
+        <v>295182910.09023738</v>
+      </c>
+      <c r="F35" s="4">
+        <f t="shared" si="6"/>
+        <v>117886854.55473545</v>
+      </c>
+      <c r="G35" s="4">
+        <f t="shared" si="6"/>
+        <v>60182919.966947541</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" si="6"/>
+        <v>311646866.70240217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" ref="A36:B36" si="7">A25</f>
+        <v>100000</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="C36" s="4">
+        <f t="shared" ref="C36:H42" si="8">($A36*$B36)/C4*1000000000</f>
+        <v>121913381.76139235</v>
+      </c>
+      <c r="D36" s="4">
+        <f t="shared" si="8"/>
+        <v>86098271.706342906</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" si="8"/>
+        <v>372688631.69232321</v>
+      </c>
+      <c r="F36" s="4">
+        <f t="shared" si="8"/>
+        <v>211725125.73825905</v>
+      </c>
+      <c r="G36" s="4">
+        <f t="shared" si="8"/>
+        <v>83310492.373340964</v>
+      </c>
+      <c r="H36" s="4">
+        <f t="shared" si="8"/>
+        <v>381303179.87786859</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f t="shared" ref="A37:B37" si="9">A26</f>
+        <v>100000</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="C37" s="4">
+        <f t="shared" si="8"/>
+        <v>226737318.01496014</v>
+      </c>
+      <c r="D37" s="4">
+        <f t="shared" si="8"/>
+        <v>88350071.254332453</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" si="8"/>
+        <v>415839319.68687296</v>
+      </c>
+      <c r="F37" s="4">
+        <f t="shared" si="8"/>
+        <v>390189846.86999458</v>
+      </c>
+      <c r="G37" s="4">
+        <f t="shared" si="8"/>
+        <v>107955132.76727059</v>
+      </c>
+      <c r="H37" s="4">
+        <f t="shared" si="8"/>
+        <v>405118264.14926177</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f t="shared" ref="A38:B38" si="10">A27</f>
+        <v>100000</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="C38" s="4">
+        <f t="shared" si="8"/>
+        <v>460453650.44776237</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" si="8"/>
+        <v>105028033.29493684</v>
+      </c>
+      <c r="E38" s="4">
+        <f t="shared" si="8"/>
+        <v>416949627.79427916</v>
+      </c>
+      <c r="F38" s="4">
+        <f t="shared" si="8"/>
+        <v>875248625.31262779</v>
+      </c>
+      <c r="G38" s="4">
+        <f t="shared" si="8"/>
+        <v>108909549.93809173</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" si="8"/>
+        <v>409161745.21805</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f t="shared" ref="A39:B39" si="11">A28</f>
+        <v>100000</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="11"/>
+        <v>16</v>
+      </c>
+      <c r="C39" s="4">
+        <f t="shared" si="8"/>
+        <v>900678267.02746332</v>
+      </c>
+      <c r="D39" s="4">
+        <f t="shared" si="8"/>
+        <v>126280563.84271754</v>
+      </c>
+      <c r="E39" s="4">
+        <f t="shared" si="8"/>
+        <v>409163105.45590872</v>
+      </c>
+      <c r="F39" s="4">
+        <f t="shared" si="8"/>
+        <v>1270032782.7212038</v>
+      </c>
+      <c r="G39" s="4">
+        <f t="shared" si="8"/>
+        <v>128573416.86748227</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" si="8"/>
+        <v>377766103.75582141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f t="shared" ref="A40:B40" si="12">A29</f>
+        <v>100000</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="12"/>
+        <v>32</v>
+      </c>
+      <c r="C40" s="4">
+        <f t="shared" si="8"/>
+        <v>1127804179.3603377</v>
+      </c>
+      <c r="D40" s="4">
+        <f t="shared" si="8"/>
+        <v>138811632.74450162</v>
+      </c>
+      <c r="E40" s="4">
+        <f t="shared" si="8"/>
+        <v>367827507.29045618</v>
+      </c>
+      <c r="F40" s="4">
+        <f t="shared" si="8"/>
+        <v>1369417484.0377276</v>
+      </c>
+      <c r="G40" s="4">
+        <f t="shared" si="8"/>
+        <v>112844098.68385696</v>
+      </c>
+      <c r="H40" s="4">
+        <f t="shared" si="8"/>
+        <v>297877002.67595947</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f t="shared" ref="A41:B41" si="13">A30</f>
+        <v>100000</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="13"/>
+        <v>64</v>
+      </c>
+      <c r="C41" s="4">
+        <f t="shared" si="8"/>
+        <v>347158542.5872131</v>
+      </c>
+      <c r="D41" s="4">
+        <f t="shared" si="8"/>
+        <v>142915511.72138318</v>
+      </c>
+      <c r="E41" s="4">
+        <f t="shared" si="8"/>
+        <v>350922405.0247702</v>
+      </c>
+      <c r="F41" s="4">
+        <f t="shared" si="8"/>
+        <v>382588150.25264865</v>
+      </c>
+      <c r="G41" s="4">
+        <f t="shared" si="8"/>
+        <v>78035904.563551888</v>
+      </c>
+      <c r="H41" s="4">
+        <f t="shared" si="8"/>
+        <v>124329161.61077598</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <f t="shared" ref="A42:B42" si="14">A31</f>
+        <v>100000</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="14"/>
+        <v>128</v>
+      </c>
+      <c r="C42" s="4">
+        <f t="shared" si="8"/>
+        <v>522366040.65721816</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="8"/>
+        <v>147872887.21846953</v>
+      </c>
+      <c r="E42" s="4">
+        <f t="shared" si="8"/>
+        <v>382974635.20095205</v>
+      </c>
+      <c r="F42" s="4">
+        <f t="shared" si="8"/>
+        <v>539434358.40330637</v>
+      </c>
+      <c r="G42" s="4">
+        <f t="shared" si="8"/>
+        <v>73763712.825487494</v>
+      </c>
+      <c r="H42" s="4">
+        <f t="shared" si="8"/>
+        <v>102931479.69607005</v>
       </c>
     </row>
   </sheetData>
@@ -35082,15 +35393,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScaleNormal="41" zoomScalePageLayoutView="41" workbookViewId="0">
-      <selection activeCell="AO3" sqref="AO3"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="74" zoomScaleNormal="41" zoomScalePageLayoutView="41" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.5" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
     <col min="4" max="4" width="23.5" customWidth="1"/>
@@ -36170,6 +36481,288 @@
         <v>0.82960063862288436</v>
       </c>
     </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C43" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <f>A33</f>
+        <v>100000</v>
+      </c>
+      <c r="B45">
+        <f>B33</f>
+        <v>1</v>
+      </c>
+      <c r="C45" s="4">
+        <f>($A45*$B45)/C2*1000000000</f>
+        <v>69752615.374313459</v>
+      </c>
+      <c r="D45" s="4">
+        <f t="shared" ref="D45:H45" si="34">($A45*$B45)/D2*1000000000</f>
+        <v>78969168.067711323</v>
+      </c>
+      <c r="E45" s="4">
+        <f t="shared" si="34"/>
+        <v>300284970.43694466</v>
+      </c>
+      <c r="F45" s="4">
+        <f t="shared" si="34"/>
+        <v>98973055.575350165</v>
+      </c>
+      <c r="G45" s="4">
+        <f t="shared" si="34"/>
+        <v>85572479.890467227</v>
+      </c>
+      <c r="H45" s="4">
+        <f t="shared" si="34"/>
+        <v>243556114.11091056</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <f t="shared" ref="A46:B46" si="35">A34</f>
+        <v>100000</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="35"/>
+        <v>2</v>
+      </c>
+      <c r="C46" s="4">
+        <f t="shared" ref="C46:H52" si="36">($A46*$B46)/C3*1000000000</f>
+        <v>143596974.98612496</v>
+      </c>
+      <c r="D46" s="4">
+        <f t="shared" si="36"/>
+        <v>103837577.26164733</v>
+      </c>
+      <c r="E46" s="4">
+        <f t="shared" si="36"/>
+        <v>371107775.26455349</v>
+      </c>
+      <c r="F46" s="4">
+        <f t="shared" si="36"/>
+        <v>219871067.60595587</v>
+      </c>
+      <c r="G46" s="4">
+        <f t="shared" si="36"/>
+        <v>121789773.79985312</v>
+      </c>
+      <c r="H46" s="4">
+        <f t="shared" si="36"/>
+        <v>311975977.84970558</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <f t="shared" ref="A47:B47" si="37">A35</f>
+        <v>100000</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="37"/>
+        <v>4</v>
+      </c>
+      <c r="C47" s="4">
+        <f t="shared" si="36"/>
+        <v>336532920.07090747</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="36"/>
+        <v>144556351.13749585</v>
+      </c>
+      <c r="E47" s="4">
+        <f t="shared" si="36"/>
+        <v>389113007.17232549</v>
+      </c>
+      <c r="F47" s="4">
+        <f t="shared" si="36"/>
+        <v>519037652.2888912</v>
+      </c>
+      <c r="G47" s="4">
+        <f t="shared" si="36"/>
+        <v>132825408.9694342</v>
+      </c>
+      <c r="H47" s="4">
+        <f t="shared" si="36"/>
+        <v>355335089.87312764</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <f t="shared" ref="A48:B48" si="38">A36</f>
+        <v>100000</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="38"/>
+        <v>8</v>
+      </c>
+      <c r="C48" s="4">
+        <f t="shared" si="36"/>
+        <v>583122255.22532213</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="36"/>
+        <v>162963524.28176883</v>
+      </c>
+      <c r="E48" s="4">
+        <f t="shared" si="36"/>
+        <v>392884083.48001009</v>
+      </c>
+      <c r="F48" s="4">
+        <f t="shared" si="36"/>
+        <v>844704284.86807299</v>
+      </c>
+      <c r="G48" s="4">
+        <f t="shared" si="36"/>
+        <v>158651619.88261765</v>
+      </c>
+      <c r="H48" s="4">
+        <f t="shared" si="36"/>
+        <v>278976310.37788391</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <f t="shared" ref="A49:B49" si="39">A37</f>
+        <v>100000</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="39"/>
+        <v>16</v>
+      </c>
+      <c r="C49" s="4">
+        <f t="shared" si="36"/>
+        <v>412031314.37989289</v>
+      </c>
+      <c r="D49" s="4">
+        <f t="shared" si="36"/>
+        <v>149267697.34145835</v>
+      </c>
+      <c r="E49" s="4">
+        <f t="shared" si="36"/>
+        <v>391374880.38605219</v>
+      </c>
+      <c r="F49" s="4">
+        <f t="shared" si="36"/>
+        <v>801679920.27293193</v>
+      </c>
+      <c r="G49" s="4">
+        <f t="shared" si="36"/>
+        <v>129681670.40366013</v>
+      </c>
+      <c r="H49" s="4">
+        <f t="shared" si="36"/>
+        <v>259264114.45992127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <f t="shared" ref="A50:B50" si="40">A38</f>
+        <v>100000</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="40"/>
+        <v>32</v>
+      </c>
+      <c r="C50" s="4">
+        <f t="shared" si="36"/>
+        <v>984821742.64822876</v>
+      </c>
+      <c r="D50" s="4">
+        <f t="shared" si="36"/>
+        <v>126691198.83368082</v>
+      </c>
+      <c r="E50" s="4">
+        <f t="shared" si="36"/>
+        <v>360206218.05983925</v>
+      </c>
+      <c r="F50" s="4">
+        <f t="shared" si="36"/>
+        <v>1063306617.7545623</v>
+      </c>
+      <c r="G50" s="4">
+        <f t="shared" si="36"/>
+        <v>105829187.39223818</v>
+      </c>
+      <c r="H50" s="4">
+        <f t="shared" si="36"/>
+        <v>305370522.75520939</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <f t="shared" ref="A51:B51" si="41">A39</f>
+        <v>100000</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="41"/>
+        <v>64</v>
+      </c>
+      <c r="C51" s="4">
+        <f t="shared" si="36"/>
+        <v>1005963793.4768906</v>
+      </c>
+      <c r="D51" s="4">
+        <f t="shared" si="36"/>
+        <v>147936188.46478665</v>
+      </c>
+      <c r="E51" s="4">
+        <f t="shared" si="36"/>
+        <v>325224470.94617349</v>
+      </c>
+      <c r="F51" s="4">
+        <f t="shared" si="36"/>
+        <v>1264601953.691462</v>
+      </c>
+      <c r="G51" s="4">
+        <f t="shared" si="36"/>
+        <v>161125258.52421853</v>
+      </c>
+      <c r="H51" s="4">
+        <f t="shared" si="36"/>
+        <v>244592003.9128606</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <f t="shared" ref="A52:B52" si="42">A40</f>
+        <v>100000</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="42"/>
+        <v>128</v>
+      </c>
+      <c r="C52" s="4">
+        <f t="shared" si="36"/>
+        <v>1537221783.8738229</v>
+      </c>
+      <c r="D52" s="4">
+        <f t="shared" si="36"/>
+        <v>165264432.38794503</v>
+      </c>
+      <c r="E52" s="4">
+        <f t="shared" si="36"/>
+        <v>310167263.51248533</v>
+      </c>
+      <c r="F52" s="4">
+        <f t="shared" si="36"/>
+        <v>1352900216.4217565</v>
+      </c>
+      <c r="G52" s="4">
+        <f t="shared" si="36"/>
+        <v>121008851.55169177</v>
+      </c>
+      <c r="H52" s="4">
+        <f t="shared" si="36"/>
+        <v>222694225.72662517</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -36180,7 +36773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>

</xml_diff>